<commit_message>
Pridani vlastni ceny a vytvoreni listu pro produkt
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Ceny" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Produkty" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,7 +439,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Medimat URL</t>
+          <t>Produkt</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -449,122 +449,97 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Produkt</t>
+          <t>Cena Heureka (Kč)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Cena Medimat (Kč)</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Cena Heureka (Kč)</t>
+          <t>Moje cena</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://eshop.medimat.cz/vlozky-tena-lady-slim-mini/</t>
+          <t>JBL Tune 720BT</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://pripravky-na-inkontinenci.heureka.cz/tena-lady-slim-mini-20-ks/#prehled/?sort-filter=lowest_price</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Tena Lady Slim Mini 20 ks</t>
-        </is>
+          <t>https://sluchatka.heureka.cz/jbl-tune-720bt/#prehled/?sort-filter=lowest_price</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>989</v>
       </c>
       <c r="E2" t="n">
-        <v>98</v>
-      </c>
-      <c r="F2" t="n">
-        <v>98</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://eshop.medimat.cz/kalhotky-zalepovaci-seni-classic-quatro-large/</t>
+          <t>JBL Tune 720BT</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://pripravky-na-inkontinenci.heureka.cz/seni-classic-quatro-l-30-ks/#prehled/?sort-filter=lowest_price</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Seni Classic Quatro L 30 ks</t>
-        </is>
+          <t>https://sluchatka.heureka.cz/jbl-tune-720bt/#prehled/?sort-filter=lowest_price</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>989</v>
       </c>
       <c r="E3" t="n">
-        <v>633</v>
-      </c>
-      <c r="F3" t="n">
-        <v>611</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://eshop.medimat.cz/kalhotky-navlekaci-tena-pants-plus-xxs/</t>
+          <t>JBL Tune 720BT</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://pripravky-na-inkontinenci.heureka.cz/tena-pants-plus-792214-xxs-14-ks/#prehled/?sort-filter=lowest_price</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Tena Pants Plus 792214 XXS 14 ks</t>
-        </is>
+          <t>https://sluchatka.heureka.cz/jbl-tune-720bt/#prehled/?sort-filter=lowest_price</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>989</v>
       </c>
       <c r="E4" t="n">
-        <v>375</v>
-      </c>
-      <c r="F4" t="n">
-        <v>371</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://eshop.medimat.cz/molicare-mobile-6-kapek-m-14-ks/</t>
+          <t>JBL Charge 6</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://pripravky-na-inkontinenci.heureka.cz/molicare-mobile-6-k-m-14-ks/#prehled/?sort-filter=lowest_price</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>MoliCare Mobile 6 k M 14 ks</t>
-        </is>
+          <t>https://bluetooth-reproduktory.heureka.cz/jbl-charge-6/#prehled/?sort-filter=lowest_price</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
       </c>
       <c r="E5" t="n">
-        <v>292</v>
-      </c>
-      <c r="F5" t="n">
-        <v>287</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>